<commit_message>
submit ss1 module 3
</commit_message>
<xml_diff>
--- a/Module2/Tài liệu/CG Audit Question Module 2.xlsx
+++ b/Module2/Tài liệu/CG Audit Question Module 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CodegymDanang\Module2\Tài liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B509AA5-7A34-4352-8318-5AB4603F870C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4729A79-E850-4F20-B1FA-C0E23AFE3A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Nội dung câu hỏi</t>
   </si>
@@ -218,14 +218,94 @@
     <t>Trình thông dịch</t>
   </si>
   <si>
-    <t>The Java™ platform is the environment for developing and managing Java applets and applications. It consists of three primary components: the Java language, the Java packages, and the Java virtual machine.</t>
+    <t>Là tập hợp các chương trình giúp chạy và phát triển và chạy các chương trình được bằng ngôn ngữ lập trình Java.
++ Java SE, Java EE, Java ME, Java FX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểu dữ liệu nguyên thuỷ: 
+byte, short, int : 0
+long: 0
+double : 0.0d
+float : 0.0f
+char: \u0000
+boolean: false
+Kiểu tham chiếu: 
+String, Array, user-defined Object : null
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stack memory:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">+ Lưu các giá trị cụ thể của các method: Các biến local và các tham chiếu tới các đối tượng chứa trong heap memory được tham chiếu bởi method.
++ Stack memory được tham chiếu theo thứ tự LIFO (Last in first out). Tức là theo stack. Khi có một method được thực thi, một block được tạo ra trong stack memory để chứa các biến nguyên thuỷ local và các tham chiếu tới các object. Khi method kết thúc, block đó sẽ không còn được sử dụng và được phục vụ cho method tiếp theo 
++ Stack có bộ nhớ nhỏ hơn nhiều so với HEAP
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Heap memory: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>+ Là bộ nhớ được sử dụng bởi Java Runtime để  cấp phát bộ nhớ cho các đối tượng (Object) và String. 
++ Bất kỳ khi nào một đối tượng được gọi, thì miền giá trị của nó sẽ được tạo lưu ở bộ nhớ HEAP
++ Bộ dọn rác (Garbage Collection) chạy trên heap memory để giải phóng bộ nhớ nếu được tượng đó không được tham chiếu tới.</t>
+    </r>
+  </si>
+  <si>
+    <t>Khai báo trước, khởi tạo sau: 
++ dataType[] arrayName;
+ -&gt; arrayName = new dataType[]{element1, element2, ...}
+Khai báo và khởi tạo cùng lúc 
+-&gt; dataTpye[] arrayName = {element1, element2, ...}</t>
+  </si>
+  <si>
+    <t>Mảng có thể lưu được nhiều kiểu dữ liệu khác nhau, tuy nhiên các phần tử trong mảng phải cùng kiểu dữ liệu (Kể cả kiểu nguyên thuỷ và tham chiếu).
++ Giá trị mặc định: 
++ null: tham chiếu
++ kiểu số nguyên: 0
++ Kiểu số thực: 0.0</t>
+  </si>
+  <si>
+    <t>Object-oriented programming: Là kĩ thuật ánh xạ những đối tượng trong thực tế vào trong lập trình.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class: 
++ Là một blueprint (Kế hoạch, bản vẽ chi tiết) hay prototype xác định properties và methods chung tất cả các đối tượng cùng loại
++ Sử dụng từ khoá class
++ Chỉ được khai báo 1 lần trong cùng 1 package
+Object: 
++ Là 1 thể hiện của class, là các đối tượng mô tả thực thể trong thế giới thực 
++ Sử dụng từ khoá new để khởi tạo
++ Đối tượng được khởi tạo nhiều lần. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -242,6 +322,32 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -441,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -464,9 +570,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
@@ -474,6 +577,12 @@
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1638,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1727,25 +1836,29 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="228" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
@@ -1756,18 +1869,22 @@
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
     </row>
@@ -1778,7 +1895,9 @@
       <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
     </row>
@@ -1789,7 +1908,9 @@
       <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
     </row>
@@ -2190,13 +2311,13 @@
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" ht="229.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="11">
+      <c r="A49" s="10">
         <v>48</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="13"/>
+      <c r="C49" s="12"/>
       <c r="D49" s="5"/>
       <c r="E49" s="6"/>
     </row>

</xml_diff>